<commit_message>
rename writeSheetRow to writeSheetCurrentRow, rewriting "per row" functions to not need to know rowcount up front, and not necessitate calling of writeSheetHead and writeSheetFooter from last nights pull request
</commit_message>
<xml_diff>
--- a/testbench/test.xlsx
+++ b/testbench/test.xlsx
@@ -33,8 +33,8 @@
   <numFmts count="4">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="[$$-1009]#,##0.00;[RED]\-[$$-1009]#,##0.00" numFmtId="165"/>
-    <numFmt formatCode="YYYY/MM/DD\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="YYYY/MM/DD" numFmtId="167"/>
+    <numFmt formatCode="YYYY-MM-DD\ HH:MM:SS" numFmtId="166"/>
+    <numFmt formatCode="YYYY-MM-DD" numFmtId="167"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -144,7 +144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A2" s="0" t="n">
         <v>2003</v>
       </c>
@@ -155,7 +155,7 @@
         <v>-50.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A3" s="0" t="n">
         <v>2003</v>
       </c>

</xml_diff>

<commit_message>
fixing "missing first row" bug
</commit_message>
<xml_diff>
--- a/testbench/test.xlsx
+++ b/testbench/test.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>year</t>
   </si>
@@ -24,6 +25,18 @@
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>first_event</t>
+  </si>
+  <si>
+    <t>second_event</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -123,7 +136,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -143,8 +156,14 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2003</v>
       </c>
@@ -154,16 +173,76 @@
       <c r="C2" s="1" t="n">
         <v>-50.5</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="D2" s="2" t="n">
+        <v>40179.958333333</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>41274</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>5</v>
+      <c r="B3" s="0" t="s">
+        <f>=B2</f>
       </c>
       <c r="C3" s="1" t="n">
         <v>23.5</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>40179</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>41274</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>343.12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>345.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>